<commit_message>
Script working apart from + sign and 2 continue buttons.
</commit_message>
<xml_diff>
--- a/src/main/resources/UserData.xlsx
+++ b/src/main/resources/UserData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25600" windowHeight="9700"/>
+    <workbookView windowWidth="25600" windowHeight="9700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
@@ -649,10 +649,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="34">
     <font>
@@ -751,6 +751,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -758,9 +765,39 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -772,23 +809,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -803,41 +826,25 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -870,24 +877,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -944,19 +944,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -968,85 +1070,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1064,13 +1094,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1082,43 +1118,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1147,6 +1147,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1162,6 +1186,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1171,17 +1210,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1203,192 +1238,157 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="20" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1706,8 +1706,8 @@
   <sheetPr/>
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1" outlineLevelCol="3"/>
@@ -2898,8 +2898,8 @@
   <sheetPr/>
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1" outlineLevelCol="3"/>
@@ -3601,9 +3601,15 @@
       <c r="A50" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="B50" s="24"/>
-      <c r="C50" s="24"/>
-      <c r="D50" s="24"/>
+      <c r="B50" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D50" s="24" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="51" ht="12.75" customHeight="1" spans="1:4">
       <c r="A51" s="24"/>

</xml_diff>